<commit_message>
Added v9 with Garki multisite multiiter calibration progress
</commit_message>
<xml_diff>
--- a/v6-Sugungum - wideParams/iter0/Cuts/500_4_W2_Sugungum/history_matching_config.xlsx
+++ b/v6-Sugungum - wideParams/iter0/Cuts/500_4_W2_Sugungum/history_matching_config.xlsx
@@ -24150,7 +24150,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.002664298401421</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -24165,7 +24165,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.03282626100881</v>
+        <v>0.3333333333333349</v>
       </c>
     </row>
     <row r="4">
@@ -24180,7 +24180,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.03284671532846</v>
+        <v>0.3333333333333329</v>
       </c>
     </row>
     <row r="5">
@@ -24195,7 +24195,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.05045871559633</v>
+        <v>0.3333333333333326</v>
       </c>
     </row>
     <row r="6">
@@ -24210,7 +24210,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.002732240437158</v>
+        <v>0.3333333333333358</v>
       </c>
     </row>
     <row r="7">
@@ -24225,7 +24225,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.09763101220386999</v>
+        <v>0.3333333333333349</v>
       </c>
     </row>
     <row r="8">
@@ -24240,7 +24240,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.06766055045871</v>
+        <v>0.3333333333333326</v>
       </c>
     </row>
     <row r="9">
@@ -24255,7 +24255,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.04753521126761</v>
+        <v>0.3333333333333352</v>
       </c>
     </row>
     <row r="10">
@@ -24270,7 +24270,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.07597851112817</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="11">
@@ -24285,7 +24285,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.09552845528455001</v>
+        <v>0.3333333333333373</v>
       </c>
     </row>
     <row r="12">
@@ -24300,7 +24300,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.07502131287297001</v>
+        <v>0.3333333333333358</v>
       </c>
     </row>
     <row r="13">
@@ -24315,7 +24315,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.12599206349206</v>
+        <v>0.3333333333333329</v>
       </c>
     </row>
     <row r="14">
@@ -24330,7 +24330,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.012135922330097</v>
+        <v>0.3333333333333351</v>
       </c>
     </row>
     <row r="15">
@@ -24345,7 +24345,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.14017094017094</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="16">
@@ -24360,7 +24360,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.07101727447216001</v>
+        <v>0.3333333333333336</v>
       </c>
     </row>
     <row r="17">
@@ -24375,7 +24375,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.08130081300813001</v>
+        <v>0.3333333333333344</v>
       </c>
     </row>
     <row r="18">
@@ -24390,7 +24390,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.04737903225807</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="19">
@@ -24405,7 +24405,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.06848184818482</v>
+        <v>0.3333333333333403</v>
       </c>
     </row>
     <row r="20">
@@ -24420,7 +24420,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.05842259006816</v>
+        <v>0.3333333333333349</v>
       </c>
     </row>
     <row r="21">
@@ -24435,7 +24435,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.09471094710948</v>
+        <v>0.3333333333333358</v>
       </c>
     </row>
     <row r="22">
@@ -24450,7 +24450,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.02834645669291</v>
+        <v>0.3333333333333349</v>
       </c>
     </row>
     <row r="23">
@@ -24465,7 +24465,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.11605584642234</v>
+        <v>0.3333333333333254</v>
       </c>
     </row>
     <row r="24">
@@ -24480,7 +24480,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.03608247422680001</v>
+        <v>0.3333333333333302</v>
       </c>
     </row>
     <row r="25">
@@ -24495,7 +24495,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.09173387096774001</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="26">
@@ -24510,7 +24510,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.020568070519096</v>
+        <v>0.3333333333333318</v>
       </c>
     </row>
     <row r="27">
@@ -24525,7 +24525,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.04597701149425</v>
+        <v>0.3333333333333379</v>
       </c>
     </row>
     <row r="28">
@@ -24540,7 +24540,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.06652360515021499</v>
+        <v>0.3333333333333359</v>
       </c>
     </row>
     <row r="29">
@@ -24555,7 +24555,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.05375139977603</v>
+        <v>0.3333333333333358</v>
       </c>
     </row>
     <row r="30">
@@ -24570,7 +24570,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.10842433697347</v>
+        <v>0.3333333333333277</v>
       </c>
     </row>
     <row r="31">
@@ -24585,7 +24585,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.119825708061</v>
+        <v>0.3333333333333337</v>
       </c>
     </row>
     <row r="32">
@@ -24600,7 +24600,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.04154863078376</v>
+        <v>0.3333333333333347</v>
       </c>
     </row>
     <row r="33">
@@ -24615,7 +24615,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.09851088201604</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="34">
@@ -24630,7 +24630,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.09327036599764001</v>
+        <v>0.3333333333333279</v>
       </c>
     </row>
     <row r="35">
@@ -24645,7 +24645,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.03873517786562</v>
+        <v>0.3333333333333323</v>
       </c>
     </row>
     <row r="36">
@@ -24660,7 +24660,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.04347826086957</v>
+        <v>0.3333333333333359</v>
       </c>
     </row>
     <row r="37">
@@ -24675,7 +24675,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.0980751604033</v>
+        <v>0.3333333333333368</v>
       </c>
     </row>
     <row r="38">
@@ -24690,7 +24690,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.03202479338843</v>
+        <v>0.3333333333333299</v>
       </c>
     </row>
     <row r="39">
@@ -24705,7 +24705,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.05644402634055001</v>
+        <v>0.333333333333331</v>
       </c>
     </row>
     <row r="40">
@@ -24720,7 +24720,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.09699999999999999</v>
+        <v>0.3333333333333347</v>
       </c>
     </row>
     <row r="41">
@@ -24735,7 +24735,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.08380952380953</v>
+        <v>0.3333333333333353</v>
       </c>
     </row>
     <row r="42">
@@ -24750,7 +24750,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.05433901054339</v>
+        <v>0.3333333333333394</v>
       </c>
     </row>
     <row r="43">
@@ -24765,7 +24765,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>0.3333333333333325</v>
       </c>
     </row>
     <row r="44">
@@ -24780,7 +24780,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.10658016682114</v>
+        <v>0.3333333333333347</v>
       </c>
     </row>
     <row r="45">
@@ -24795,7 +24795,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.04938271604937999</v>
+        <v>0.33333333333334</v>
       </c>
     </row>
     <row r="46">
@@ -24810,7 +24810,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.08289703315882001</v>
+        <v>0.3333333333333332</v>
       </c>
     </row>
     <row r="47">
@@ -24825,7 +24825,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.14352720450282</v>
+        <v>0.3333333333333367</v>
       </c>
     </row>
     <row r="48">
@@ -24840,7 +24840,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.039637599094</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="49">
@@ -24855,7 +24855,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.11849390919158</v>
+        <v>0.3333333333333355</v>
       </c>
     </row>
     <row r="50">
@@ -24870,7 +24870,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.10578842315369</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="51">
@@ -24885,7 +24885,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.06388206388206999</v>
+        <v>0.3333333333333339</v>
       </c>
     </row>
     <row r="52">
@@ -24900,7 +24900,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.02653525398029</v>
+        <v>0.3333333333333325</v>
       </c>
     </row>
     <row r="53">
@@ -24915,7 +24915,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.029940119760474</v>
+        <v>0.3333333333333332</v>
       </c>
     </row>
     <row r="54">
@@ -24930,7 +24930,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.07580174927114</v>
+        <v>0.3333333333333389</v>
       </c>
     </row>
     <row r="55">
@@ -24945,7 +24945,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.11759172154281</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="56">
@@ -24960,7 +24960,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.01578947368421</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="57">
@@ -24975,7 +24975,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.03427895981087</v>
+        <v>0.3333333333333261</v>
       </c>
     </row>
     <row r="58">
@@ -24990,7 +24990,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.07663197729422999</v>
+        <v>0.3333333333333297</v>
       </c>
     </row>
     <row r="59">
@@ -25005,7 +25005,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.021297192642788</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="60">
@@ -25020,7 +25020,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.01289566236811</v>
+        <v>0.3333333333333354</v>
       </c>
     </row>
     <row r="61">
@@ -25035,7 +25035,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.12987012987013</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="62">
@@ -25050,7 +25050,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.02800908402726</v>
+        <v>0.3333333333333318</v>
       </c>
     </row>
     <row r="63">
@@ -25065,7 +25065,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.16888888888888</v>
+        <v>0.3333333333333284</v>
       </c>
     </row>
     <row r="64">
@@ -25080,7 +25080,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.15603448275862</v>
+        <v>0.3333333333333297</v>
       </c>
     </row>
     <row r="65">
@@ -25095,7 +25095,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.12778603268945</v>
+        <v>0.3333333333333369</v>
       </c>
     </row>
     <row r="66">
@@ -25110,7 +25110,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.04302925989673</v>
+        <v>0.3333333333333309</v>
       </c>
     </row>
     <row r="67">
@@ -25125,7 +25125,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.018722466960352</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="68">
@@ -25140,7 +25140,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.004664179104477999</v>
+        <v>0.3333333333333381</v>
       </c>
     </row>
     <row r="69">
@@ -25155,7 +25155,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.05955555555556</v>
+        <v>0.3333333333333363</v>
       </c>
     </row>
     <row r="70">
@@ -25170,7 +25170,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.09485714285715</v>
+        <v>0.3333333333333342</v>
       </c>
     </row>
     <row r="71">
@@ -25185,7 +25185,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.05532617671346</v>
+        <v>0.3333333333333369</v>
       </c>
     </row>
     <row r="72">
@@ -25200,7 +25200,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.019178082191783</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="73">
@@ -25215,7 +25215,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.05382215288612001</v>
+        <v>0.3333333333333341</v>
       </c>
     </row>
     <row r="74">
@@ -25230,7 +25230,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.06399132321041999</v>
+        <v>0.3333333333333351</v>
       </c>
     </row>
     <row r="75">
@@ -25245,7 +25245,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.05454545454545</v>
+        <v>0.3333333333333363</v>
       </c>
     </row>
     <row r="76">
@@ -25260,7 +25260,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.07814045499505999</v>
+        <v>0.333333333333334</v>
       </c>
     </row>
     <row r="77">
@@ -25275,7 +25275,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.0039331366764999</v>
+        <v>0.3333333333333344</v>
       </c>
     </row>
     <row r="78">
@@ -25290,7 +25290,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.06415396952685999</v>
+        <v>0.3333333333333356</v>
       </c>
     </row>
     <row r="79">
@@ -25305,7 +25305,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.06765067650676999</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="80">
@@ -25320,7 +25320,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.05179982440738</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="81">
@@ -25335,7 +25335,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0.021233569261877</v>
+        <v>0.3333333333333328</v>
       </c>
     </row>
     <row r="82">
@@ -25350,7 +25350,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.030156815440288</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="83">
@@ -25365,7 +25365,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.06613756613756999</v>
+        <v>0.3333333333333225</v>
       </c>
     </row>
     <row r="84">
@@ -25380,7 +25380,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.04434589800444001</v>
+        <v>0.3333333333333397</v>
       </c>
     </row>
     <row r="85">
@@ -25395,7 +25395,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.05591397849463001</v>
+        <v>0.3333333333333328</v>
       </c>
     </row>
     <row r="86">
@@ -25410,7 +25410,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0.09323583180988</v>
+        <v>0.3333333333333369</v>
       </c>
     </row>
     <row r="87">
@@ -25425,7 +25425,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.03803888419273</v>
+        <v>0.3333333333333358</v>
       </c>
     </row>
     <row r="88">
@@ -25440,7 +25440,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.06646294881589</v>
+        <v>0.3333333333333353</v>
       </c>
     </row>
     <row r="89">
@@ -25455,7 +25455,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.05633802816902</v>
+        <v>0.3333333333333326</v>
       </c>
     </row>
     <row r="90">
@@ -25470,7 +25470,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.014705882352944</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="91">
@@ -25485,7 +25485,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.13888888888892</v>
+        <v>0.3333333333333364</v>
       </c>
     </row>
     <row r="92">
@@ -25500,7 +25500,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.08882521489971</v>
+        <v>0.3333333333333328</v>
       </c>
     </row>
     <row r="93">
@@ -25515,7 +25515,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.04512195121951</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="94">
@@ -25530,7 +25530,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.06990881458967001</v>
+        <v>0.3333333333333311</v>
       </c>
     </row>
     <row r="95">
@@ -25545,7 +25545,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.10282574568288</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="96">
@@ -25560,7 +25560,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.13639788997738</v>
+        <v>0.3333333333333336</v>
       </c>
     </row>
     <row r="97">
@@ -25575,7 +25575,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0.0038610038610038</v>
+        <v>0.3333333333333294</v>
       </c>
     </row>
     <row r="98">
@@ -25590,7 +25590,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.08546168958742999</v>
+        <v>0.3333333333333323</v>
       </c>
     </row>
     <row r="99">
@@ -25605,7 +25605,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0.01190476190476</v>
+        <v>0.3333333333333407</v>
       </c>
     </row>
     <row r="100">
@@ -25620,7 +25620,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0.03608247422680001</v>
+        <v>0.3333333333333358</v>
       </c>
     </row>
     <row r="101">
@@ -25635,7 +25635,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0.18909710391823</v>
+        <v>0.3333333333333305</v>
       </c>
     </row>
     <row r="102">
@@ -25650,7 +25650,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0.14738805970149</v>
+        <v>0.333333333333336</v>
       </c>
     </row>
     <row r="103">
@@ -25665,7 +25665,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.03750000000000001</v>
+        <v>0.3333333333333314</v>
       </c>
     </row>
     <row r="104">
@@ -25680,7 +25680,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0.04022988505747</v>
+        <v>0.3333333333333272</v>
       </c>
     </row>
     <row r="105">
@@ -25695,7 +25695,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>0.04012841091493299</v>
+        <v>0.333333333333331</v>
       </c>
     </row>
     <row r="106">
@@ -25710,7 +25710,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0.09775784753363</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="107">
@@ -25725,7 +25725,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>0.1082995951417</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="108">
@@ -25740,7 +25740,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0.05808823529411</v>
+        <v>0.3333333333333307</v>
       </c>
     </row>
     <row r="109">
@@ -25755,7 +25755,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>0.11957796014068</v>
+        <v>0.3333333333333326</v>
       </c>
     </row>
     <row r="110">
@@ -25770,7 +25770,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>0.04594594594595</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="111">
@@ -25785,7 +25785,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>0.06563706563707</v>
+        <v>0.3333333333333339</v>
       </c>
     </row>
     <row r="112">
@@ -25800,7 +25800,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>0.09214092140922001</v>
+        <v>0.3333333333333364</v>
       </c>
     </row>
     <row r="113">
@@ -25815,7 +25815,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0.03324099722991999</v>
+        <v>0.3333333333333337</v>
       </c>
     </row>
     <row r="114">
@@ -25830,7 +25830,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>0.0395809080326</v>
+        <v>0.333333333333337</v>
       </c>
     </row>
     <row r="115">
@@ -25845,7 +25845,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0.14814814814815</v>
+        <v>0.3333333333333386</v>
       </c>
     </row>
     <row r="116">
@@ -25860,7 +25860,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0.05447470817121</v>
+        <v>0.3333333333333387</v>
       </c>
     </row>
     <row r="117">
@@ -25875,7 +25875,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>0.06999125109361999</v>
+        <v>0.3333333333333327</v>
       </c>
     </row>
     <row r="118">
@@ -25890,7 +25890,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>0.05004549590537</v>
+        <v>0.3333333333333354</v>
       </c>
     </row>
     <row r="119">
@@ -25905,7 +25905,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0.16375</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="120">
@@ -25920,7 +25920,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>0.07398568019092999</v>
+        <v>0.3333333333333317</v>
       </c>
     </row>
     <row r="121">
@@ -25935,7 +25935,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>0.04114713216957</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="122">
@@ -25950,7 +25950,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>0.12718204488778</v>
+        <v>0.3333333333333401</v>
       </c>
     </row>
     <row r="123">
@@ -25965,7 +25965,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>0.09985096870342</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="124">
@@ -25980,7 +25980,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>0.05471478463330001</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="125">
@@ -25995,7 +25995,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>0.05016722408027</v>
+        <v>0.3333333333333369</v>
       </c>
     </row>
     <row r="126">
@@ -26010,7 +26010,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0.10724106324473</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="127">
@@ -26025,7 +26025,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0.05281285878301</v>
+        <v>0.333333333333331</v>
       </c>
     </row>
     <row r="128">
@@ -26040,7 +26040,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>0.04468599033816</v>
+        <v>0.333333333333334</v>
       </c>
     </row>
     <row r="129">
@@ -26055,7 +26055,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>0</v>
+        <v>0.3333333333333273</v>
       </c>
     </row>
     <row r="130">
@@ -26070,7 +26070,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0.05656759348035</v>
+        <v>0.3333333333333343</v>
       </c>
     </row>
     <row r="131">
@@ -26085,7 +26085,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>0.06225680933852999</v>
+        <v>0.3333333333333365</v>
       </c>
     </row>
     <row r="132">
@@ -26100,7 +26100,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0.09198813056379</v>
+        <v>0.333333333333329</v>
       </c>
     </row>
     <row r="133">
@@ -26115,7 +26115,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.012422360248451</v>
+        <v>0.3333333333333323</v>
       </c>
     </row>
     <row r="134">
@@ -26130,7 +26130,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>0.06690454950937</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="135">
@@ -26145,7 +26145,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0.06311637080868</v>
+        <v>0.3333333333333308</v>
       </c>
     </row>
     <row r="136">
@@ -26160,7 +26160,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>0.06893106893107001</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="137">
@@ -26175,7 +26175,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>0.19672131147542</v>
+        <v>0.3333333333333385</v>
       </c>
     </row>
     <row r="138">
@@ -26190,7 +26190,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>0.04518828451882</v>
+        <v>0.3333333333333336</v>
       </c>
     </row>
     <row r="139">
@@ -26205,7 +26205,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>0.15604681404421</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="140">
@@ -26220,7 +26220,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0.04734299516909</v>
+        <v>0.3333333333333298</v>
       </c>
     </row>
     <row r="141">
@@ -26235,7 +26235,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0.03252885624344</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="142">
@@ -26250,7 +26250,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0.08311688311689</v>
+        <v>0.3333333333333353</v>
       </c>
     </row>
     <row r="143">
@@ -26265,7 +26265,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>0.0438521066208</v>
+        <v>0.3333333333333302</v>
       </c>
     </row>
     <row r="144">
@@ -26280,7 +26280,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>0.05228031145718</v>
+        <v>0.3333333333333336</v>
       </c>
     </row>
     <row r="145">
@@ -26295,7 +26295,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>0.04886877828054</v>
+        <v>0.3333333333333259</v>
       </c>
     </row>
     <row r="146">
@@ -26310,7 +26310,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>0.09554140127388</v>
+        <v>0.333333333333324</v>
       </c>
     </row>
     <row r="147">
@@ -26325,7 +26325,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>0.04837117472853</v>
+        <v>0.3333333333333353</v>
       </c>
     </row>
     <row r="148">
@@ -26340,7 +26340,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>0.02941176470588</v>
+        <v>0.3333333333333361</v>
       </c>
     </row>
     <row r="149">
@@ -26355,7 +26355,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>0.05189620758483</v>
+        <v>0.3333333333333302</v>
       </c>
     </row>
     <row r="150">
@@ -26370,7 +26370,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>0.05640423031728</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="151">
@@ -26385,7 +26385,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>0.07623318385651</v>
+        <v>0.3333333333333356</v>
       </c>
     </row>
     <row r="152">
@@ -26400,7 +26400,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0.08180943214629</v>
+        <v>0.3333333333333243</v>
       </c>
     </row>
     <row r="153">
@@ -26415,7 +26415,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>0.16525423728812</v>
+        <v>0.3333333333333367</v>
       </c>
     </row>
     <row r="154">
@@ -26430,7 +26430,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>0.036963036963039</v>
+        <v>0.333333333333332</v>
       </c>
     </row>
     <row r="155">
@@ -26445,7 +26445,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>0.10308285163776</v>
+        <v>0.3333333333333376</v>
       </c>
     </row>
     <row r="156">
@@ -26460,7 +26460,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0.014285714285711</v>
+        <v>0.3333333333333315</v>
       </c>
     </row>
     <row r="157">
@@ -26475,7 +26475,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>0.06981981981982001</v>
+        <v>0.333333333333329</v>
       </c>
     </row>
     <row r="158">
@@ -26490,7 +26490,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>0.04472271914132</v>
+        <v>0.3333333333333325</v>
       </c>
     </row>
     <row r="159">
@@ -26505,7 +26505,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>0.09358974358974001</v>
+        <v>0.3333333333333366</v>
       </c>
     </row>
     <row r="160">
@@ -26520,7 +26520,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>0.05357142857143</v>
+        <v>0.3333333333333293</v>
       </c>
     </row>
     <row r="161">
@@ -26535,7 +26535,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0.08074534161491001</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="162">
@@ -26550,7 +26550,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>0.03721488595439</v>
+        <v>0.3333333333333355</v>
       </c>
     </row>
     <row r="163">
@@ -26565,7 +26565,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>0.06631097560976</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="164">
@@ -26580,7 +26580,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>0.06418918918919</v>
+        <v>0.3333333333333337</v>
       </c>
     </row>
     <row r="165">
@@ -26595,7 +26595,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>0.06317411402158001</v>
+        <v>0.3333333333333356</v>
       </c>
     </row>
     <row r="166">
@@ -26610,7 +26610,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>0.05268490374873</v>
+        <v>0.3333333333333313</v>
       </c>
     </row>
     <row r="167">
@@ -26625,7 +26625,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>0.06486486486487</v>
+        <v>0.333333333333332</v>
       </c>
     </row>
     <row r="168">
@@ -26640,7 +26640,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>0</v>
+        <v>0.3333333333333318</v>
       </c>
     </row>
     <row r="169">
@@ -26655,7 +26655,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>0.013908205841447</v>
+        <v>0.3333333333333351</v>
       </c>
     </row>
     <row r="170">
@@ -26670,7 +26670,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>0.12086330935252</v>
+        <v>0.3333333333333318</v>
       </c>
     </row>
     <row r="171">
@@ -26685,7 +26685,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>0.10750507099392</v>
+        <v>0.3333333333333393</v>
       </c>
     </row>
     <row r="172">
@@ -26700,7 +26700,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>0.03677758318739</v>
+        <v>0.3333333333333378</v>
       </c>
     </row>
     <row r="173">
@@ -26715,7 +26715,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>0.03921568627451</v>
+        <v>0.3333333333333253</v>
       </c>
     </row>
     <row r="174">
@@ -26730,7 +26730,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>0.07387140902872999</v>
+        <v>0.333333333333338</v>
       </c>
     </row>
     <row r="175">
@@ -26745,7 +26745,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>0.07911683532658001</v>
+        <v>0.333333333333334</v>
       </c>
     </row>
     <row r="176">
@@ -26760,7 +26760,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>0.04552715654952</v>
+        <v>0.333333333333327</v>
       </c>
     </row>
     <row r="177">
@@ -26775,7 +26775,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>0.07361963190184001</v>
+        <v>0.3333333333333395</v>
       </c>
     </row>
     <row r="178">
@@ -26790,7 +26790,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>0.168421052631579</v>
+        <v>0.3333333333333322</v>
       </c>
     </row>
     <row r="179">
@@ -26805,7 +26805,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>0.05343511450380999</v>
+        <v>0.3333333333333359</v>
       </c>
     </row>
     <row r="180">
@@ -26820,7 +26820,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>0.01450443190975</v>
+        <v>0.3333333333333366</v>
       </c>
     </row>
     <row r="181">
@@ -26835,7 +26835,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>0.013771186440678</v>
+        <v>0.3333333333333338</v>
       </c>
     </row>
     <row r="182">
@@ -26850,7 +26850,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>0.018882769472856</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="183">
@@ -26865,7 +26865,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>0.1110065851364</v>
+        <v>0.3333333333333318</v>
       </c>
     </row>
     <row r="184">
@@ -26880,7 +26880,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>0.0565371024735</v>
+        <v>0.3333333333333305</v>
       </c>
     </row>
     <row r="185">
@@ -26895,7 +26895,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>0.0682261208577</v>
+        <v>0.3333333333333396</v>
       </c>
     </row>
     <row r="186">
@@ -26910,7 +26910,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>0.05168269230769</v>
+        <v>0.3333333333333305</v>
       </c>
     </row>
     <row r="187">
@@ -26925,7 +26925,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>0.09320388349514</v>
+        <v>0.3333333333333349</v>
       </c>
     </row>
     <row r="188">
@@ -26940,7 +26940,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>0.06076854334226999</v>
+        <v>0.3333333333333341</v>
       </c>
     </row>
     <row r="189">
@@ -26955,7 +26955,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>0.030864197530863</v>
+        <v>0.3333333333333347</v>
       </c>
     </row>
     <row r="190">
@@ -26970,7 +26970,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>0.06563706563706001</v>
+        <v>0.3333333333333366</v>
       </c>
     </row>
     <row r="191">
@@ -26985,7 +26985,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>0.12899896800825</v>
+        <v>0.3333333333333332</v>
       </c>
     </row>
     <row r="192">
@@ -27000,7 +27000,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>0.04570895522388</v>
+        <v>0.3333333333333376</v>
       </c>
     </row>
     <row r="193">
@@ -27015,7 +27015,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>0.018726591760298</v>
+        <v>0.3333333333333303</v>
       </c>
     </row>
     <row r="194">
@@ -27030,7 +27030,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>0.09297052154195</v>
+        <v>0.3333333333333393</v>
       </c>
     </row>
     <row r="195">
@@ -27045,7 +27045,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>0.09553571428572001</v>
+        <v>0.3333333333333393</v>
       </c>
     </row>
     <row r="196">
@@ -27060,7 +27060,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>0.08355978260869999</v>
+        <v>0.3333333333333306</v>
       </c>
     </row>
     <row r="197">
@@ -27075,7 +27075,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>0.015459723352319</v>
+        <v>0.3333333333333366</v>
       </c>
     </row>
     <row r="198">
@@ -27090,7 +27090,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>0.09722222222222</v>
+        <v>0.3333333333333383</v>
       </c>
     </row>
     <row r="199">
@@ -27105,7 +27105,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>0.05609284332689</v>
+        <v>0.3333333333333336</v>
       </c>
     </row>
     <row r="200">
@@ -27120,7 +27120,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>0.06026200873362</v>
+        <v>0.3333333333333344</v>
       </c>
     </row>
     <row r="201">
@@ -27135,7 +27135,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>0.15062287655719</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="202">
@@ -27150,7 +27150,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>0.05</v>
+        <v>0.3333333333333312</v>
       </c>
     </row>
     <row r="203">
@@ -27165,7 +27165,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>0.07671601615074</v>
+        <v>0.3333333333333328</v>
       </c>
     </row>
     <row r="204">
@@ -27180,7 +27180,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>0.05045492142267</v>
+        <v>0.3333333333333351</v>
       </c>
     </row>
     <row r="205">
@@ -27195,7 +27195,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>0.08898776418242001</v>
+        <v>0.3333333333333373</v>
       </c>
     </row>
     <row r="206">
@@ -27210,7 +27210,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>0.03775411423039</v>
+        <v>0.3333333333333312</v>
       </c>
     </row>
     <row r="207">
@@ -27225,7 +27225,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>0.09779179810726001</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="208">
@@ -27240,7 +27240,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>0.15571428571429</v>
+        <v>0.3333333333333355</v>
       </c>
     </row>
     <row r="209">
@@ -27255,7 +27255,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>0.08685162846803</v>
+        <v>0.333333333333329</v>
       </c>
     </row>
     <row r="210">
@@ -27270,7 +27270,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>0.13997113997113</v>
+        <v>0.3333333333333327</v>
       </c>
     </row>
     <row r="211">
@@ -27285,7 +27285,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>0.0008733624454148</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="212">
@@ -27300,7 +27300,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>0.08004385964913001</v>
+        <v>0.3333333333333301</v>
       </c>
     </row>
     <row r="213">
@@ -27315,7 +27315,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>0.02734375</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="214">
@@ -27330,7 +27330,7 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>0.03622497616778</v>
+        <v>0.3333333333333336</v>
       </c>
     </row>
     <row r="215">
@@ -27345,7 +27345,7 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>0.12990007686395</v>
+        <v>0.3333333333333383</v>
       </c>
     </row>
     <row r="216">
@@ -27360,7 +27360,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>0.03460514640639</v>
+        <v>0.3333333333333366</v>
       </c>
     </row>
     <row r="217">
@@ -27375,7 +27375,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>0.08981481481480999</v>
+        <v>0.3333333333333345</v>
       </c>
     </row>
     <row r="218">
@@ -27390,7 +27390,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>0.07274590163935001</v>
+        <v>0.3333333333333305</v>
       </c>
     </row>
     <row r="219">
@@ -27405,7 +27405,7 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>0.08362369337978999</v>
+        <v>0.3333333333333294</v>
       </c>
     </row>
     <row r="220">
@@ -27420,7 +27420,7 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>0.11111111111111</v>
+        <v>0.333333333333329</v>
       </c>
     </row>
     <row r="221">
@@ -27435,7 +27435,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>0.08282208588956999</v>
+        <v>0.3333333333333328</v>
       </c>
     </row>
     <row r="222">
@@ -27450,7 +27450,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>0.09332260659694001</v>
+        <v>0.3333333333333363</v>
       </c>
     </row>
     <row r="223">
@@ -27465,7 +27465,7 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>0.10454545454546</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="224">
@@ -27480,7 +27480,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>0.05823627287853</v>
+        <v>0.3333333333333345</v>
       </c>
     </row>
     <row r="225">
@@ -27495,7 +27495,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>0.08098271155596001</v>
+        <v>0.3333333333333381</v>
       </c>
     </row>
     <row r="226">
@@ -27510,7 +27510,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>0.017706576728502</v>
+        <v>0.3333333333333345</v>
       </c>
     </row>
     <row r="227">
@@ -27525,7 +27525,7 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>0.06085918854415</v>
+        <v>0.3333333333333372</v>
       </c>
     </row>
     <row r="228">
@@ -27540,7 +27540,7 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>0.04244604316547</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="229">
@@ -27555,7 +27555,7 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>0.003208556149732999</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="230">
@@ -27570,7 +27570,7 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>0.04484304932736</v>
+        <v>0.3333333333333294</v>
       </c>
     </row>
     <row r="231">
@@ -27585,7 +27585,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>0.08603491271819999</v>
+        <v>0.3333333333333369</v>
       </c>
     </row>
     <row r="232">
@@ -27600,7 +27600,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>0.02941176470588</v>
+        <v>0.3333333333333375</v>
       </c>
     </row>
     <row r="233">
@@ -27615,7 +27615,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>0.08953817153627999</v>
+        <v>0.3333333333333372</v>
       </c>
     </row>
     <row r="234">
@@ -27630,7 +27630,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>0.04397705544933</v>
+        <v>0.3333333333333361</v>
       </c>
     </row>
     <row r="235">
@@ -27645,7 +27645,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>0.06135770234987</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="236">
@@ -27660,7 +27660,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>0.07698289269052001</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="237">
@@ -27675,7 +27675,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>0.19246861924687</v>
+        <v>0.3333333333333355</v>
       </c>
     </row>
     <row r="238">
@@ -27690,7 +27690,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>0.013574660633484</v>
+        <v>0.3333333333333325</v>
       </c>
     </row>
     <row r="239">
@@ -27705,7 +27705,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>0.06811145510836</v>
+        <v>0.3333333333333371</v>
       </c>
     </row>
     <row r="240">
@@ -27720,7 +27720,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>0.10264227642276</v>
+        <v>0.3333333333333277</v>
       </c>
     </row>
     <row r="241">
@@ -27735,7 +27735,7 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>0.017295597484276</v>
+        <v>0.3333333333333296</v>
       </c>
     </row>
     <row r="242">
@@ -27750,7 +27750,7 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>0.006910167818361001</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="243">
@@ -27765,7 +27765,7 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>0.14431082331179</v>
+        <v>0.333333333333336</v>
       </c>
     </row>
     <row r="244">
@@ -27780,7 +27780,7 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>0.04442581726739001</v>
+        <v>0.3333333333333371</v>
       </c>
     </row>
     <row r="245">
@@ -27795,7 +27795,7 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>0.08364451082897001</v>
+        <v>0.333333333333332</v>
       </c>
     </row>
     <row r="246">
@@ -27810,7 +27810,7 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>0.02457002457002</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="247">
@@ -27825,7 +27825,7 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>0.06514657980456</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="248">
@@ -27840,7 +27840,7 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>0.08333333333333001</v>
+        <v>0.3333333333333285</v>
       </c>
     </row>
     <row r="249">
@@ -27855,7 +27855,7 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>0.10888888888889</v>
+        <v>0.3333333333333345</v>
       </c>
     </row>
     <row r="250">
@@ -27870,7 +27870,7 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>0.05714285714286001</v>
+        <v>0.3333333333333288</v>
       </c>
     </row>
     <row r="251">
@@ -27885,7 +27885,7 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>0.03885480572597001</v>
+        <v>0.3333333333333359</v>
       </c>
     </row>
     <row r="252">
@@ -27900,7 +27900,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>0.06368821292776</v>
+        <v>0.3333333333333318</v>
       </c>
     </row>
     <row r="253">
@@ -27915,7 +27915,7 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>0.13786764705882</v>
+        <v>0.3333333333333361</v>
       </c>
     </row>
     <row r="254">
@@ -27930,7 +27930,7 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>0.08247422680413</v>
+        <v>0.3333333333333396</v>
       </c>
     </row>
     <row r="255">
@@ -27945,7 +27945,7 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>0.09492273730685001</v>
+        <v>0.3333333333333314</v>
       </c>
     </row>
     <row r="256">
@@ -27960,7 +27960,7 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>0.11770943796395</v>
+        <v>0.333333333333331</v>
       </c>
     </row>
     <row r="257">
@@ -27975,7 +27975,7 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>0.06518723994452</v>
+        <v>0.3333333333333343</v>
       </c>
     </row>
     <row r="258">
@@ -27990,7 +27990,7 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>0.04166666666667</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="259">
@@ -28005,7 +28005,7 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>0.05745721271394</v>
+        <v>0.3333333333333301</v>
       </c>
     </row>
     <row r="260">
@@ -28020,7 +28020,7 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>0.05084745762712</v>
+        <v>0.333333333333332</v>
       </c>
     </row>
     <row r="261">
@@ -28035,7 +28035,7 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>0.04651162790698</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="262">
@@ -28050,7 +28050,7 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>0.02804487179488</v>
+        <v>0.3333333333333346</v>
       </c>
     </row>
     <row r="263">
@@ -28065,7 +28065,7 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>0.08196721311475999</v>
+        <v>0.3333333333333359</v>
       </c>
     </row>
     <row r="264">
@@ -28080,7 +28080,7 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>0.06538049303323</v>
+        <v>0.3333333333333429</v>
       </c>
     </row>
     <row r="265">
@@ -28095,7 +28095,7 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>0.05939393939394</v>
+        <v>0.3333333333333336</v>
       </c>
     </row>
     <row r="266">
@@ -28110,7 +28110,7 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>0.04234527687297</v>
+        <v>0.3333333333333342</v>
       </c>
     </row>
     <row r="267">
@@ -28125,7 +28125,7 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>0.13254310344827</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="268">
@@ -28140,7 +28140,7 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>0.07783882783883</v>
+        <v>0.3333333333333305</v>
       </c>
     </row>
     <row r="269">
@@ -28155,7 +28155,7 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>0.05357142857143</v>
+        <v>0.3333333333333318</v>
       </c>
     </row>
     <row r="270">
@@ -28170,7 +28170,7 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>0.0763358778626</v>
+        <v>0.3333333333333325</v>
       </c>
     </row>
     <row r="271">
@@ -28185,7 +28185,7 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>0.0523560209424</v>
+        <v>0.3333333333333353</v>
       </c>
     </row>
     <row r="272">
@@ -28200,7 +28200,7 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>0.03330411919369</v>
+        <v>0.3333333333333369</v>
       </c>
     </row>
     <row r="273">
@@ -28215,7 +28215,7 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>0.11055900621118</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="274">
@@ -28230,7 +28230,7 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>0.04588014981273</v>
+        <v>0.3333333333333304</v>
       </c>
     </row>
     <row r="275">
@@ -28245,7 +28245,7 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>0.004024144869215</v>
+        <v>0.3333333333333276</v>
       </c>
     </row>
     <row r="276">
@@ -28260,7 +28260,7 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>0.07994579945800001</v>
+        <v>0.3333333333333342</v>
       </c>
     </row>
     <row r="277">
@@ -28275,7 +28275,7 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>0.127783155856687</v>
+        <v>0.3333333333333287</v>
       </c>
     </row>
     <row r="278">
@@ -28290,7 +28290,7 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>0.03491271820448</v>
+        <v>0.333333333333332</v>
       </c>
     </row>
     <row r="279">
@@ -28305,7 +28305,7 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>0</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="280">
@@ -28320,7 +28320,7 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>0.0802752293578</v>
+        <v>0.3333333333333349</v>
       </c>
     </row>
     <row r="281">
@@ -28335,7 +28335,7 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>0.015984015984013</v>
+        <v>0.3333333333333383</v>
       </c>
     </row>
     <row r="282">
@@ -28350,7 +28350,7 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>0.07801418439716</v>
+        <v>0.3333333333333298</v>
       </c>
     </row>
     <row r="283">
@@ -28365,7 +28365,7 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>0.03389830508475</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="284">
@@ -28380,7 +28380,7 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>0.06631016042781</v>
+        <v>0.3333333333333306</v>
       </c>
     </row>
     <row r="285">
@@ -28395,7 +28395,7 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>0.04032258064516001</v>
+        <v>0.3333333333333368</v>
       </c>
     </row>
     <row r="286">
@@ -28410,7 +28410,7 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>0.06043046357615001</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="287">
@@ -28425,7 +28425,7 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>0.1317907444668</v>
+        <v>0.3333333333333338</v>
       </c>
     </row>
     <row r="288">
@@ -28440,7 +28440,7 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>0.13628762541806</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="289">
@@ -28455,7 +28455,7 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>0.07795473595975999</v>
+        <v>0.3333333333333339</v>
       </c>
     </row>
     <row r="290">
@@ -28470,7 +28470,7 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>0.05189620758484</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="291">
@@ -28485,7 +28485,7 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>0.05795148247979001</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="292">
@@ -28500,7 +28500,7 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>0.06717226435536</v>
+        <v>0.3333333333333337</v>
       </c>
     </row>
     <row r="293">
@@ -28515,7 +28515,7 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>0.023111111111113</v>
+        <v>0.3333333333333358</v>
       </c>
     </row>
     <row r="294">
@@ -28530,7 +28530,7 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>0.01544401544402</v>
+        <v>0.3333333333333328</v>
       </c>
     </row>
     <row r="295">
@@ -28545,7 +28545,7 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>0.05413687436159</v>
+        <v>0.3333333333333344</v>
       </c>
     </row>
     <row r="296">
@@ -28560,7 +28560,7 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>0.04404145077721</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="297">
@@ -28575,7 +28575,7 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>0.03026315789473</v>
+        <v>0.3333333333333252</v>
       </c>
     </row>
     <row r="298">
@@ -28590,7 +28590,7 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>0.12456344586728</v>
+        <v>0.333333333333336</v>
       </c>
     </row>
     <row r="299">
@@ -28605,7 +28605,7 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>0.05248618784530001</v>
+        <v>0.3333333333333306</v>
       </c>
     </row>
     <row r="300">
@@ -28620,7 +28620,7 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>0.12650602409639</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="301">
@@ -28635,7 +28635,7 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>0.06148590947907</v>
+        <v>0.3333333333333313</v>
       </c>
     </row>
     <row r="302">
@@ -28650,7 +28650,7 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>0.0625</v>
+        <v>0.3333333333333369</v>
       </c>
     </row>
     <row r="303">
@@ -28665,7 +28665,7 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>0.04670558798998999</v>
+        <v>0.3333333333333352</v>
       </c>
     </row>
     <row r="304">
@@ -28680,7 +28680,7 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>0.006939090208173001</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="305">
@@ -28695,7 +28695,7 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>0.1332744924978</v>
+        <v>0.3333333333333296</v>
       </c>
     </row>
     <row r="306">
@@ -28710,7 +28710,7 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>0.012182741116752</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="307">
@@ -28725,7 +28725,7 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>0.07340720221605999</v>
+        <v>0.3333333333333344</v>
       </c>
     </row>
     <row r="308">
@@ -28740,7 +28740,7 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>0.09846650524617</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="309">
@@ -28755,7 +28755,7 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>0.02096985583224</v>
+        <v>0.3333333333333322</v>
       </c>
     </row>
     <row r="310">
@@ -28770,7 +28770,7 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>0.05924596050269</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="311">
@@ -28785,7 +28785,7 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>0.10201249132547</v>
+        <v>0.3333333333333299</v>
       </c>
     </row>
     <row r="312">
@@ -28800,7 +28800,7 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>0</v>
+        <v>0.3333333333333338</v>
       </c>
     </row>
     <row r="313">
@@ -28815,7 +28815,7 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>0.13384955752216</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="314">
@@ -28830,7 +28830,7 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>0.07349397590361201</v>
+        <v>0.3333333333333295</v>
       </c>
     </row>
     <row r="315">
@@ -28845,7 +28845,7 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>0.12801678908709</v>
+        <v>0.3333333333333299</v>
       </c>
     </row>
     <row r="316">
@@ -28860,7 +28860,7 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>0.001204819277108</v>
+        <v>0.3333333333333323</v>
       </c>
     </row>
     <row r="317">
@@ -28875,7 +28875,7 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>0.17142857142855</v>
+        <v>0.3333333333333373</v>
       </c>
     </row>
     <row r="318">
@@ -28890,7 +28890,7 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>0.07990012484393999</v>
+        <v>0.3333333333333368</v>
       </c>
     </row>
     <row r="319">
@@ -28905,7 +28905,7 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>0.10253807106599</v>
+        <v>0.3333333333333367</v>
       </c>
     </row>
     <row r="320">
@@ -28920,7 +28920,7 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>0.04179104477612</v>
+        <v>0.3333333333333329</v>
       </c>
     </row>
     <row r="321">
@@ -28935,7 +28935,7 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>0.15254237288134</v>
+        <v>0.333333333333328</v>
       </c>
     </row>
     <row r="322">
@@ -28950,7 +28950,7 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>0.08251231527094</v>
+        <v>0.3333333333333308</v>
       </c>
     </row>
     <row r="323">
@@ -28965,7 +28965,7 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>0.14324817518248</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="324">
@@ -28980,7 +28980,7 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>0.028571428571427</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="325">
@@ -28995,7 +28995,7 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>0.05833333333333</v>
+        <v>0.3333333333333303</v>
       </c>
     </row>
     <row r="326">
@@ -29010,7 +29010,7 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>0.05045278137128</v>
+        <v>0.3333333333333299</v>
       </c>
     </row>
     <row r="327">
@@ -29025,7 +29025,7 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>0.023917995444187</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="328">
@@ -29040,7 +29040,7 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>0.07552650689906</v>
+        <v>0.3333333333333325</v>
       </c>
     </row>
     <row r="329">
@@ -29055,7 +29055,7 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>0.04112149532711</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="330">
@@ -29070,7 +29070,7 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>0.06259541984733</v>
+        <v>0.3333333333333361</v>
       </c>
     </row>
     <row r="331">
@@ -29085,7 +29085,7 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>0.10526315789474</v>
+        <v>0.333333333333337</v>
       </c>
     </row>
     <row r="332">
@@ -29100,7 +29100,7 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>0.1494042163153</v>
+        <v>0.3333333333333362</v>
       </c>
     </row>
     <row r="333">
@@ -29115,7 +29115,7 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>0</v>
+        <v>0.3333333333333318</v>
       </c>
     </row>
     <row r="334">
@@ -29130,7 +29130,7 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>0.11182336182336</v>
+        <v>0.3333333333333317</v>
       </c>
     </row>
     <row r="335">
@@ -29145,7 +29145,7 @@
         </is>
       </c>
       <c r="C335" t="n">
-        <v>0.024447031431899</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="336">
@@ -29160,7 +29160,7 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>0.07724867724866999</v>
+        <v>0.3333333333333288</v>
       </c>
     </row>
     <row r="337">
@@ -29175,7 +29175,7 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>0.05807814149947</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="338">
@@ -29190,7 +29190,7 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>0.08644610458912</v>
+        <v>0.3333333333333298</v>
       </c>
     </row>
     <row r="339">
@@ -29205,7 +29205,7 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>0.0464135021097</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="340">
@@ -29220,7 +29220,7 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>0.06303236797274001</v>
+        <v>0.333333333333336</v>
       </c>
     </row>
     <row r="341">
@@ -29235,7 +29235,7 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>0.05628373168851</v>
+        <v>0.3333333333333351</v>
       </c>
     </row>
     <row r="342">
@@ -29250,7 +29250,7 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>0.07582515611061999</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="343">
@@ -29265,7 +29265,7 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>0.07789678675755</v>
+        <v>0.333333333333332</v>
       </c>
     </row>
     <row r="344">
@@ -29280,7 +29280,7 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>0.03400174367917</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="345">
@@ -29295,7 +29295,7 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>0.1015873015873</v>
+        <v>0.33333333333333</v>
       </c>
     </row>
     <row r="346">
@@ -29310,7 +29310,7 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>0.07568238213399001</v>
+        <v>0.3333333333333279</v>
       </c>
     </row>
     <row r="347">
@@ -29325,7 +29325,7 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>0.02835249042146</v>
+        <v>0.3333333333333403</v>
       </c>
     </row>
     <row r="348">
@@ -29340,7 +29340,7 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>0.007623888182974</v>
+        <v>0.3333333333333435</v>
       </c>
     </row>
     <row r="349">
@@ -29355,7 +29355,7 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>0.040072859745</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="350">
@@ -29370,7 +29370,7 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>0.07276736493936001</v>
+        <v>0.3333333333333339</v>
       </c>
     </row>
     <row r="351">
@@ -29385,7 +29385,7 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>0.06581352833637999</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="352">
@@ -29400,7 +29400,7 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>0.12929292929293</v>
+        <v>0.3333333333333254</v>
       </c>
     </row>
     <row r="353">
@@ -29415,7 +29415,7 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>0.0383631713555</v>
+        <v>0.3333333333333396</v>
       </c>
     </row>
     <row r="354">
@@ -29430,7 +29430,7 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>0.020725388601041</v>
+        <v>0.3333333333333322</v>
       </c>
     </row>
     <row r="355">
@@ -29445,7 +29445,7 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>0.08947804473903001</v>
+        <v>0.3333333333333345</v>
       </c>
     </row>
     <row r="356">
@@ -29460,7 +29460,7 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>0.07243816254416999</v>
+        <v>0.3333333333333367</v>
       </c>
     </row>
     <row r="357">
@@ -29475,7 +29475,7 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>0.08060453400504</v>
+        <v>0.3333333333333301</v>
       </c>
     </row>
     <row r="358">
@@ -29490,7 +29490,7 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>0.06776180698152</v>
+        <v>0.3333333333333346</v>
       </c>
     </row>
     <row r="359">
@@ -29505,7 +29505,7 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>0.09183673469387001</v>
+        <v>0.3333333333333308</v>
       </c>
     </row>
     <row r="360">
@@ -29520,7 +29520,7 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>0.04039301310043</v>
+        <v>0.3333333333333366</v>
       </c>
     </row>
     <row r="361">
@@ -29535,7 +29535,7 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>0.06189967982924999</v>
+        <v>0.3333333333333368</v>
       </c>
     </row>
     <row r="362">
@@ -29550,7 +29550,7 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>0.013344453711427</v>
+        <v>0.3333333333333365</v>
       </c>
     </row>
     <row r="363">
@@ -29565,7 +29565,7 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>0.06916426512967999</v>
+        <v>0.3333333333333389</v>
       </c>
     </row>
     <row r="364">
@@ -29580,7 +29580,7 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>0.004884856943475</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="365">
@@ -29595,7 +29595,7 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>0.14525139664804</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="366">
@@ -29610,7 +29610,7 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>0.12674418604651</v>
+        <v>0.3333333333333314</v>
       </c>
     </row>
     <row r="367">
@@ -29625,7 +29625,7 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>0.05830039525691001</v>
+        <v>0.3333333333333326</v>
       </c>
     </row>
     <row r="368">
@@ -29640,7 +29640,7 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>0.09111791730475</v>
+        <v>0.3333333333333306</v>
       </c>
     </row>
     <row r="369">
@@ -29655,7 +29655,7 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>0.00705329153605</v>
+        <v>0.333333333333334</v>
       </c>
     </row>
     <row r="370">
@@ -29670,7 +29670,7 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>0.08064516129032001</v>
+        <v>0.3333333333333342</v>
       </c>
     </row>
     <row r="371">
@@ -29685,7 +29685,7 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>0.09350057012542</v>
+        <v>0.3333333333333351</v>
       </c>
     </row>
     <row r="372">
@@ -29700,7 +29700,7 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>0.06613047363717001</v>
+        <v>0.3333333333333309</v>
       </c>
     </row>
     <row r="373">
@@ -29715,7 +29715,7 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>0.08605664488017001</v>
+        <v>0.3333333333333327</v>
       </c>
     </row>
     <row r="374">
@@ -29730,7 +29730,7 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>0.02937576499389</v>
+        <v>0.3333333333333313</v>
       </c>
     </row>
     <row r="375">
@@ -29745,7 +29745,7 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>0.08571428571428</v>
+        <v>0.3333333333333247</v>
       </c>
     </row>
     <row r="376">
@@ -29760,7 +29760,7 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>0.08925750394943999</v>
+        <v>0.3333333333333345</v>
       </c>
     </row>
     <row r="377">
@@ -29775,7 +29775,7 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>0.075382803298</v>
+        <v>0.3333333333333294</v>
       </c>
     </row>
     <row r="378">
@@ -29790,7 +29790,7 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>0.018214936247725</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="379">
@@ -29805,7 +29805,7 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>0.07205623901582001</v>
+        <v>0.3333333333333372</v>
       </c>
     </row>
     <row r="380">
@@ -29820,7 +29820,7 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>0.016236867239734</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="381">
@@ -29835,7 +29835,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>0.031639501438163</v>
+        <v>0.3333333333333338</v>
       </c>
     </row>
     <row r="382">
@@ -29850,7 +29850,7 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>0.06280667320903</v>
+        <v>0.3333333333333371</v>
       </c>
     </row>
     <row r="383">
@@ -29865,7 +29865,7 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>0.05543933054393</v>
+        <v>0.3333333333333332</v>
       </c>
     </row>
     <row r="384">
@@ -29880,7 +29880,7 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>0.07783955520253999</v>
+        <v>0.3333333333333374</v>
       </c>
     </row>
     <row r="385">
@@ -29895,7 +29895,7 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>0.02391496899912</v>
+        <v>0.3333333333333326</v>
       </c>
     </row>
     <row r="386">
@@ -29910,7 +29910,7 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>0.04208416833667</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="387">
@@ -29925,7 +29925,7 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>0.05081157374734999</v>
+        <v>0.3333333333333361</v>
       </c>
     </row>
     <row r="388">
@@ -29940,7 +29940,7 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>0.022047244094493</v>
+        <v>0.3333333333333356</v>
       </c>
     </row>
     <row r="389">
@@ -29955,7 +29955,7 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>0.036240090600231</v>
+        <v>0.3333333333333381</v>
       </c>
     </row>
     <row r="390">
@@ -29970,7 +29970,7 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>0.024800708591679</v>
+        <v>0.3333333333333327</v>
       </c>
     </row>
     <row r="391">
@@ -29985,7 +29985,7 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>0.16346153846159</v>
+        <v>0.3333333333333338</v>
       </c>
     </row>
     <row r="392">
@@ -30000,7 +30000,7 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>0.07162790697674</v>
+        <v>0.3333333333333345</v>
       </c>
     </row>
     <row r="393">
@@ -30015,7 +30015,7 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>0.06828811973807</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="394">
@@ -30030,7 +30030,7 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>0.04672897196261</v>
+        <v>0.3333333333333339</v>
       </c>
     </row>
     <row r="395">
@@ -30045,7 +30045,7 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>0.00418410041841</v>
+        <v>0.3333333333333328</v>
       </c>
     </row>
     <row r="396">
@@ -30060,7 +30060,7 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>0.075</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="397">
@@ -30075,7 +30075,7 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>0.05011933174223999</v>
+        <v>0.3333333333333305</v>
       </c>
     </row>
     <row r="398">
@@ -30090,7 +30090,7 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>0.06986190089357999</v>
+        <v>0.3333333333333339</v>
       </c>
     </row>
     <row r="399">
@@ -30105,7 +30105,7 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>0.07489878542510001</v>
+        <v>0.3333333333333395</v>
       </c>
     </row>
     <row r="400">
@@ -30120,7 +30120,7 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>0.06661786237188999</v>
+        <v>0.3333333333333411</v>
       </c>
     </row>
     <row r="401">
@@ -30135,7 +30135,7 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>0.07253886010362</v>
+        <v>0.3333333333333312</v>
       </c>
     </row>
     <row r="402">
@@ -30150,7 +30150,7 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>0.03843648208469</v>
+        <v>0.333333333333332</v>
       </c>
     </row>
     <row r="403">
@@ -30165,7 +30165,7 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>0.04545454545455</v>
+        <v>0.3333333333333305</v>
       </c>
     </row>
     <row r="404">
@@ -30180,7 +30180,7 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>0.07438016528925001</v>
+        <v>0.333333333333332</v>
       </c>
     </row>
     <row r="405">
@@ -30195,7 +30195,7 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>0.03498542274051999</v>
+        <v>0.3333333333333369</v>
       </c>
     </row>
     <row r="406">
@@ -30210,7 +30210,7 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>0.01127819548872</v>
+        <v>0.3333333333333326</v>
       </c>
     </row>
     <row r="407">
@@ -30225,7 +30225,7 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>0.08894230769230999</v>
+        <v>0.3333333333333373</v>
       </c>
     </row>
     <row r="408">
@@ -30240,7 +30240,7 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>0.11198120595145</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="409">
@@ -30255,7 +30255,7 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>0.05579868708972</v>
+        <v>0.3333333333333302</v>
       </c>
     </row>
     <row r="410">
@@ -30270,7 +30270,7 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>0.08494208494208999</v>
+        <v>0.3333333333333287</v>
       </c>
     </row>
     <row r="411">
@@ -30285,7 +30285,7 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>0.05816554809844</v>
+        <v>0.3333333333333357</v>
       </c>
     </row>
     <row r="412">
@@ -30300,7 +30300,7 @@
         </is>
       </c>
       <c r="C412" t="n">
-        <v>0.05684210526316</v>
+        <v>0.3333333333333374</v>
       </c>
     </row>
     <row r="413">
@@ -30315,7 +30315,7 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>0.13354700854701</v>
+        <v>0.3333333333333323</v>
       </c>
     </row>
     <row r="414">
@@ -30330,7 +30330,7 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>0.06504065040649999</v>
+        <v>0.3333333333333399</v>
       </c>
     </row>
     <row r="415">
@@ -30345,7 +30345,7 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>0.0528233151184</v>
+        <v>0.3333333333333323</v>
       </c>
     </row>
     <row r="416">
@@ -30360,7 +30360,7 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>0.12180746561886</v>
+        <v>0.3333333333333352</v>
       </c>
     </row>
     <row r="417">
@@ -30375,7 +30375,7 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>0.07370517928287</v>
+        <v>0.3333333333333301</v>
       </c>
     </row>
     <row r="418">
@@ -30390,7 +30390,7 @@
         </is>
       </c>
       <c r="C418" t="n">
-        <v>0.08272251308900999</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="419">
@@ -30405,7 +30405,7 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>0.07479508196721001</v>
+        <v>0.3333333333333282</v>
       </c>
     </row>
     <row r="420">
@@ -30420,7 +30420,7 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>0.05900151285931</v>
+        <v>0.3333333333333355</v>
       </c>
     </row>
     <row r="421">
@@ -30435,7 +30435,7 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>0.016057091882248</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="422">
@@ -30450,7 +30450,7 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>0.06807511737089</v>
+        <v>0.3333333333333353</v>
       </c>
     </row>
     <row r="423">
@@ -30465,7 +30465,7 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>0.08616780045352</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="424">
@@ -30480,7 +30480,7 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>0.05890052356021</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="425">
@@ -30495,7 +30495,7 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>0.02875695732839</v>
+        <v>0.333333333333334</v>
       </c>
     </row>
     <row r="426">
@@ -30510,7 +30510,7 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>0.03366762177651</v>
+        <v>0.3333333333333336</v>
       </c>
     </row>
     <row r="427">
@@ -30525,7 +30525,7 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>0.021359223300972</v>
+        <v>0.3333333333333314</v>
       </c>
     </row>
     <row r="428">
@@ -30540,7 +30540,7 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>0.016853932584268</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="429">
@@ -30555,7 +30555,7 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>0.09100529100529001</v>
+        <v>0.3333333333333341</v>
       </c>
     </row>
     <row r="430">
@@ -30570,7 +30570,7 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>0.09357652656621</v>
+        <v>0.3333333333333326</v>
       </c>
     </row>
     <row r="431">
@@ -30585,7 +30585,7 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>0.03901046622265</v>
+        <v>0.3333333333333329</v>
       </c>
     </row>
     <row r="432">
@@ -30600,7 +30600,7 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>0.03617571059432</v>
+        <v>0.333333333333338</v>
       </c>
     </row>
     <row r="433">
@@ -30615,7 +30615,7 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>0.1187707641196</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="434">
@@ -30630,7 +30630,7 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>0.09544468546638001</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="435">
@@ -30645,7 +30645,7 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>0.04375896700144</v>
+        <v>0.3333333333333368</v>
       </c>
     </row>
     <row r="436">
@@ -30660,7 +30660,7 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>0.04048964218456</v>
+        <v>0.333333333333337</v>
       </c>
     </row>
     <row r="437">
@@ -30675,7 +30675,7 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>0.03918722786647</v>
+        <v>0.3333333333333343</v>
       </c>
     </row>
     <row r="438">
@@ -30690,7 +30690,7 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>0.09104938271605</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="439">
@@ -30705,7 +30705,7 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>0.05992509363296</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="440">
@@ -30720,7 +30720,7 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>0.014522821576761</v>
+        <v>0.3333333333333263</v>
       </c>
     </row>
     <row r="441">
@@ -30735,7 +30735,7 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>0.09971910112360001</v>
+        <v>0.3333333333333297</v>
       </c>
     </row>
     <row r="442">
@@ -30750,7 +30750,7 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>0.07355679702048</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="443">
@@ -30765,7 +30765,7 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>0</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="444">
@@ -30780,7 +30780,7 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>0.04418985270050001</v>
+        <v>0.3333333333333311</v>
       </c>
     </row>
     <row r="445">
@@ -30795,7 +30795,7 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>0.08935742971888</v>
+        <v>0.3333333333333255</v>
       </c>
     </row>
     <row r="446">
@@ -30810,7 +30810,7 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>0.07337278106509</v>
+        <v>0.3333333333333346</v>
       </c>
     </row>
     <row r="447">
@@ -30825,7 +30825,7 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>0.1084452975048</v>
+        <v>0.3333333333333311</v>
       </c>
     </row>
     <row r="448">
@@ -30840,7 +30840,7 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>0</v>
+        <v>0.3333333333333355</v>
       </c>
     </row>
     <row r="449">
@@ -30855,7 +30855,7 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>0.0793499043977</v>
+        <v>0.333333333333335</v>
       </c>
     </row>
     <row r="450">
@@ -30870,7 +30870,7 @@
         </is>
       </c>
       <c r="C450" t="n">
-        <v>0.03291384317522</v>
+        <v>0.333333333333336</v>
       </c>
     </row>
     <row r="451">
@@ -30885,7 +30885,7 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>0.04831358249772</v>
+        <v>0.3333333333333297</v>
       </c>
     </row>
     <row r="452">
@@ -30900,7 +30900,7 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>0.06882591093116999</v>
+        <v>0.3333333333333311</v>
       </c>
     </row>
     <row r="453">
@@ -30915,7 +30915,7 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>0.08602150537635</v>
+        <v>0.3333333333333309</v>
       </c>
     </row>
     <row r="454">
@@ -30930,7 +30930,7 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>0.13048368953881</v>
+        <v>0.3333333333333304</v>
       </c>
     </row>
     <row r="455">
@@ -30945,7 +30945,7 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>0.0059473237043326</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="456">
@@ -30960,7 +30960,7 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>0.036625971143176</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="457">
@@ -30975,7 +30975,7 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>0.022482014388487</v>
+        <v>0.3333333333333393</v>
       </c>
     </row>
     <row r="458">
@@ -30990,7 +30990,7 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>0.04963680387409</v>
+        <v>0.3333333333333328</v>
       </c>
     </row>
     <row r="459">
@@ -31005,7 +31005,7 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>0.024334600760453</v>
+        <v>0.3333333333333315</v>
       </c>
     </row>
     <row r="460">
@@ -31020,7 +31020,7 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>0.04887983706721</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="461">
@@ -31035,7 +31035,7 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>0.07855251544572001</v>
+        <v>0.3333333333333322</v>
       </c>
     </row>
     <row r="462">
@@ -31050,7 +31050,7 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>0.01527614571093</v>
+        <v>0.3333333333333307</v>
       </c>
     </row>
     <row r="463">
@@ -31065,7 +31065,7 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>0.03908484270733999</v>
+        <v>0.3333333333333352</v>
       </c>
     </row>
     <row r="464">
@@ -31080,7 +31080,7 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>0.03670745272525</v>
+        <v>0.3333333333333312</v>
       </c>
     </row>
     <row r="465">
@@ -31095,7 +31095,7 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>0.15358744394615</v>
+        <v>0.3333333333333305</v>
       </c>
     </row>
     <row r="466">
@@ -31110,7 +31110,7 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>0</v>
+        <v>0.3333333333333325</v>
       </c>
     </row>
     <row r="467">
@@ -31125,7 +31125,7 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>0.05870646766169001</v>
+        <v>0.3333333333333389</v>
       </c>
     </row>
     <row r="468">
@@ -31140,7 +31140,7 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>0.07623318385651</v>
+        <v>0.3333333333333257</v>
       </c>
     </row>
     <row r="469">
@@ -31155,7 +31155,7 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>0.04020100502513</v>
+        <v>0.3333333333333336</v>
       </c>
     </row>
     <row r="470">
@@ -31170,7 +31170,7 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>0.05633802816901</v>
+        <v>0.3333333333333268</v>
       </c>
     </row>
     <row r="471">
@@ -31185,7 +31185,7 @@
         </is>
       </c>
       <c r="C471" t="n">
-        <v>0.07392996108949001</v>
+        <v>0.3333333333333298</v>
       </c>
     </row>
     <row r="472">
@@ -31200,7 +31200,7 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>0.17476635514021</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="473">
@@ -31215,7 +31215,7 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>0.06933333333333</v>
+        <v>0.333333333333334</v>
       </c>
     </row>
     <row r="474">
@@ -31230,7 +31230,7 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>0.12948207171314</v>
+        <v>0.3333333333333323</v>
       </c>
     </row>
     <row r="475">
@@ -31245,7 +31245,7 @@
         </is>
       </c>
       <c r="C475" t="n">
-        <v>0.04829857299671</v>
+        <v>0.3333333333333316</v>
       </c>
     </row>
     <row r="476">
@@ -31260,7 +31260,7 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>0.02990033222591</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="477">
@@ -31275,7 +31275,7 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>0.15101645692163</v>
+        <v>0.3333333333333303</v>
       </c>
     </row>
     <row r="478">
@@ -31290,7 +31290,7 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>0.12946428571428</v>
+        <v>0.3333333333333341</v>
       </c>
     </row>
     <row r="479">
@@ -31305,7 +31305,7 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>0.08791208791208999</v>
+        <v>0.3333333333333347</v>
       </c>
     </row>
     <row r="480">
@@ -31320,7 +31320,7 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>0.05</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="481">
@@ -31335,7 +31335,7 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>0.08823529411764999</v>
+        <v>0.3333333333333328</v>
       </c>
     </row>
     <row r="482">
@@ -31350,7 +31350,7 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>0.01663585951941</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="483">
@@ -31365,7 +31365,7 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>0.03121387283237</v>
+        <v>0.3333333333333324</v>
       </c>
     </row>
     <row r="484">
@@ -31380,7 +31380,7 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>0.10958904109589</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="485">
@@ -31395,7 +31395,7 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>0.06636155606407</v>
+        <v>0.3333333333333245</v>
       </c>
     </row>
     <row r="486">
@@ -31410,7 +31410,7 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>0.04116222760291</v>
+        <v>0.333333333333325</v>
       </c>
     </row>
     <row r="487">
@@ -31425,7 +31425,7 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>0.016441005802708</v>
+        <v>0.3333333333333343</v>
       </c>
     </row>
     <row r="488">
@@ -31440,7 +31440,7 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>0.07704654895666001</v>
+        <v>0.3333333333333346</v>
       </c>
     </row>
     <row r="489">
@@ -31455,7 +31455,7 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>0.07329401853412</v>
+        <v>0.3333333333333366</v>
       </c>
     </row>
     <row r="490">
@@ -31470,7 +31470,7 @@
         </is>
       </c>
       <c r="C490" t="n">
-        <v>0.04493392070483999</v>
+        <v>0.333333333333334</v>
       </c>
     </row>
     <row r="491">
@@ -31485,7 +31485,7 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>0.05475763016158001</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="492">
@@ -31500,7 +31500,7 @@
         </is>
       </c>
       <c r="C492" t="n">
-        <v>0.09495798319328001</v>
+        <v>0.3333333333333345</v>
       </c>
     </row>
     <row r="493">
@@ -31515,7 +31515,7 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>0.05269607843137</v>
+        <v>0.3333333333333318</v>
       </c>
     </row>
     <row r="494">
@@ -31530,7 +31530,7 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>0.04843110504775</v>
+        <v>0.3333333333333308</v>
       </c>
     </row>
     <row r="495">
@@ -31545,7 +31545,7 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>0.09147424511545001</v>
+        <v>0.3333333333333302</v>
       </c>
     </row>
     <row r="496">
@@ -31560,7 +31560,7 @@
         </is>
       </c>
       <c r="C496" t="n">
-        <v>0.08187134502924001</v>
+        <v>0.3333333333333374</v>
       </c>
     </row>
     <row r="497">
@@ -31575,7 +31575,7 @@
         </is>
       </c>
       <c r="C497" t="n">
-        <v>0.14558303886926</v>
+        <v>0.333333333333334</v>
       </c>
     </row>
     <row r="498">
@@ -31590,7 +31590,7 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>0.07511737089202</v>
+        <v>0.3333333333333273</v>
       </c>
     </row>
     <row r="499">
@@ -31605,7 +31605,7 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>0.09417398244213999</v>
+        <v>0.3333333333333337</v>
       </c>
     </row>
     <row r="500">
@@ -31620,7 +31620,7 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>0.027154663518297</v>
+        <v>0.3333333333333369</v>
       </c>
     </row>
     <row r="501">
@@ -31635,7 +31635,7 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>0.04887983706721</v>
+        <v>0.3333333333333332</v>
       </c>
     </row>
     <row r="502">
@@ -31650,7 +31650,7 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>0.07415036045314</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="503">
@@ -31665,7 +31665,7 @@
         </is>
       </c>
       <c r="C503" t="n">
-        <v>0.03309203722855</v>
+        <v>0.3333333333333331</v>
       </c>
     </row>
     <row r="504">
@@ -31680,7 +31680,7 @@
         </is>
       </c>
       <c r="C504" t="n">
-        <v>0.05395683453237</v>
+        <v>0.3333333333333321</v>
       </c>
     </row>
     <row r="505">
@@ -31695,7 +31695,7 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>0.024557956777999</v>
+        <v>0.3333333333333342</v>
       </c>
     </row>
     <row r="506">
@@ -31710,7 +31710,7 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>0.07770270270269999</v>
+        <v>0.3333333333333379</v>
       </c>
     </row>
     <row r="507">
@@ -31725,7 +31725,7 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>0.11133603238867</v>
+        <v>0.3333333333333292</v>
       </c>
     </row>
     <row r="508">
@@ -31740,7 +31740,7 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>0.1336170212766</v>
+        <v>0.3333333333333317</v>
       </c>
     </row>
     <row r="509">
@@ -31755,7 +31755,7 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>0.008310249307479001</v>
+        <v>0.3333333333333346</v>
       </c>
     </row>
     <row r="510">
@@ -31770,7 +31770,7 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>0.10263929618769</v>
+        <v>0.3333333333333319</v>
       </c>
     </row>
     <row r="511">
@@ -31785,7 +31785,7 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>0.04771573604061</v>
+        <v>0.3333333333333344</v>
       </c>
     </row>
     <row r="512">
@@ -31800,7 +31800,7 @@
         </is>
       </c>
       <c r="C512" t="n">
-        <v>0.08029197080292</v>
+        <v>0.3333333333333348</v>
       </c>
     </row>
     <row r="513">
@@ -31815,7 +31815,7 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>0.15618860510806</v>
+        <v>0.3333333333333374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>